<commit_message>
SOM clustering implemented, yet to be analyzed :)
</commit_message>
<xml_diff>
--- a/results/resumenOnlyMet.xlsx
+++ b/results/resumenOnlyMet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="191">
   <si>
     <t>clustersResumen</t>
   </si>
@@ -317,9 +317,6 @@
     <t xml:space="preserve">En los datos antropométricos vemos que el peso, el IMC y la grasa se ven influenciados por el endulzante, la grasa por todos los factores y el IRCV por el tiempo y el sexo. </t>
   </si>
   <si>
-    <t>2-way</t>
-  </si>
-  <si>
     <t>ST</t>
   </si>
   <si>
@@ -369,13 +366,247 @@
   </si>
   <si>
     <t xml:space="preserve">0.000539 </t>
+  </si>
+  <si>
+    <t>0.00000113</t>
+  </si>
+  <si>
+    <t>0.008</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>0.003</t>
+  </si>
+  <si>
+    <t>sucralosa menos para hombres?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0000428 </t>
+  </si>
+  <si>
+    <t>0.000169</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.038</t>
+  </si>
+  <si>
+    <t>0.000000588</t>
+  </si>
+  <si>
+    <t>0.029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.023 </t>
+  </si>
+  <si>
+    <t>0.032</t>
+  </si>
+  <si>
+    <t>0.047</t>
+  </si>
+  <si>
+    <t>1????</t>
+  </si>
+  <si>
+    <t>0.035</t>
+  </si>
+  <si>
+    <t>0.000967</t>
+  </si>
+  <si>
+    <t>0.039</t>
+  </si>
+  <si>
+    <t>0.009</t>
+  </si>
+  <si>
+    <t>0.000937</t>
+  </si>
+  <si>
+    <t>0.000201</t>
+  </si>
+  <si>
+    <t>Bpmin no-sig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.036 </t>
+  </si>
+  <si>
+    <t>Frec no sig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El CA.Gluc en comparaciones múltiples sale casi 1 en p-valor, y aquí sale muy claramente influenciado por el tiempo </t>
+  </si>
+  <si>
+    <t>0.037</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.019 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0000772 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0000995 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.006 </t>
+  </si>
+  <si>
+    <t>0.000121</t>
+  </si>
+  <si>
+    <t>0.000234</t>
+  </si>
+  <si>
+    <t>0.007</t>
+  </si>
+  <si>
+    <t>0.017</t>
+  </si>
+  <si>
+    <t>0.000233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0000524 </t>
+  </si>
+  <si>
+    <t>Todos los valores metabólicos no significativos</t>
+  </si>
+  <si>
+    <t>0.0000000103</t>
+  </si>
+  <si>
+    <t>5.97e-4</t>
+  </si>
+  <si>
+    <t>2.9 e-2</t>
+  </si>
+  <si>
+    <t>1.3 e-2</t>
+  </si>
+  <si>
+    <t>6   e-3</t>
+  </si>
+  <si>
+    <t>3.64e-5</t>
+  </si>
+  <si>
+    <t>7   e-3</t>
+  </si>
+  <si>
+    <t>2   e-3</t>
+  </si>
+  <si>
+    <t>8.67e-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.74e-4 </t>
+  </si>
+  <si>
+    <t>0.015</t>
+  </si>
+  <si>
+    <t>0.012</t>
+  </si>
+  <si>
+    <t>0.046</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.009</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X3.4.Ácido.Dihidroxifenilacético..DHPAA.</t>
+  </si>
+  <si>
+    <t>8.79e-5</t>
+  </si>
+  <si>
+    <t>0.036</t>
+  </si>
+  <si>
+    <t>1.09e-6</t>
+  </si>
+  <si>
+    <t>0.0000678</t>
+  </si>
+  <si>
+    <t>4.43e-4</t>
+  </si>
+  <si>
+    <t>5.62e-4</t>
+  </si>
+  <si>
+    <t>0.0000357</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VA.GG</t>
+  </si>
+  <si>
+    <t>0.0000000378</t>
+  </si>
+  <si>
+    <t>0.0000413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004 </t>
+  </si>
+  <si>
+    <t>0.000000342</t>
+  </si>
+  <si>
+    <t>0.00000648</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.001</t>
+  </si>
+  <si>
+    <t>0.000102</t>
+  </si>
+  <si>
+    <t>0.0000425</t>
+  </si>
+  <si>
+    <t>0.000192</t>
+  </si>
+  <si>
+    <t>0.000544</t>
+  </si>
+  <si>
+    <t>0.000406</t>
+  </si>
+  <si>
+    <t>0.000556</t>
+  </si>
+  <si>
+    <t>0.045</t>
+  </si>
+  <si>
+    <t>0.025</t>
+  </si>
+  <si>
+    <t>0.038</t>
+  </si>
+  <si>
+    <t>Conclusiones</t>
+  </si>
+  <si>
+    <t>Valores metabolicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En orinaFlav </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -417,8 +648,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,6 +759,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -797,7 +1059,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -868,10 +1130,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T84"/>
+  <dimension ref="A1:T87"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67:K67"/>
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -2399,6 +2671,11 @@
     <row r="84" spans="1:1">
       <c r="A84" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2420,285 +2697,1712 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G27"/>
+  <dimension ref="A2:AB65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" spans="1:28">
+      <c r="B2" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="72" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="C3" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="J3" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="Q3" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="X3" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="71"/>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="B4" s="70" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="C3" s="66" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R4" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S4" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T4" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U4" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="W4" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="X4" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y4" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z4" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA4" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB4" s="68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="F4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="66" t="s">
+      <c r="H5" s="69"/>
+      <c r="I5" t="s">
+        <v>188</v>
+      </c>
+      <c r="O5" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="P5" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="R5" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="S5" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="T5" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="U5" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="V5" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="W5" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y5" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z5" s="63"/>
+      <c r="AA5" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB5" s="63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" s="73"/>
+      <c r="B6" s="68" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="66"/>
-      <c r="B6" t="s">
-        <v>101</v>
       </c>
       <c r="F6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" t="s">
+      <c r="H6" s="69"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q6" s="63" t="s">
+        <v>153</v>
+      </c>
+      <c r="R6" s="63" t="s">
+        <v>152</v>
+      </c>
+      <c r="T6" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="V6" s="73"/>
+      <c r="W6" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y6" s="63"/>
+      <c r="AA6" s="63"/>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" s="73"/>
+      <c r="B7" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
         <v>104</v>
       </c>
-      <c r="C7" t="s">
+      <c r="H7" s="69"/>
+      <c r="I7" t="s">
+        <v>189</v>
+      </c>
+      <c r="O7" s="73"/>
+      <c r="P7" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q7" s="63" t="s">
+        <v>156</v>
+      </c>
+      <c r="R7" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="S7" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="V7" s="73"/>
+      <c r="W7" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z7" s="63"/>
+    </row>
+    <row r="8" spans="1:28">
+      <c r="C8" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="I8" t="s">
+        <v>190</v>
+      </c>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="Q8" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+    </row>
+    <row r="9" spans="1:28">
+      <c r="B9" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R9" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S9" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T9" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U9" s="68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28">
+      <c r="A10" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="69"/>
+      <c r="O10" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="R10" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="T10" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="U10" s="63" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28">
+      <c r="A11" s="73"/>
+      <c r="B11" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="69"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="68" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28">
+      <c r="A12" s="73"/>
+      <c r="B12" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="C8" s="66" t="s">
+      <c r="H12" s="69"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="S12" s="63" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28">
+      <c r="C13" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="66"/>
-      <c r="B11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="C13" s="66" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
       <c r="G13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="69"/>
+      <c r="Q13" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" s="71"/>
+      <c r="S13" s="71"/>
+      <c r="T13" s="71"/>
+      <c r="U13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28">
+      <c r="B14" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
+      <c r="P14" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q14" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R14" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S14" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T14" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U14" s="63" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28">
+      <c r="A15" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="F14" t="s">
-        <v>104</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" t="s">
-        <v>108</v>
       </c>
       <c r="F15" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="66"/>
-      <c r="B16" t="s">
-        <v>101</v>
+      <c r="H15" s="69"/>
+      <c r="O15" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q15" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="R15" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="S15" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="T15" s="63" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28">
+      <c r="A16" s="73"/>
+      <c r="B16" s="68" t="s">
+        <v>100</v>
       </c>
       <c r="E16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="69"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="68" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="73"/>
+      <c r="B17" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
         <v>109</v>
       </c>
-      <c r="F16" t="s">
+      <c r="D17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="69"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q17" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="S17" s="63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="C18" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="Q18" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R18" s="71"/>
+      <c r="S18" s="71"/>
+      <c r="T18" s="71"/>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="B19" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="48"/>
+      <c r="P19" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="R19" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="S19" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="T19" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="U19" s="67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="63" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="63" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
+      <c r="H20" s="69"/>
+      <c r="O20" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="S20" s="63" t="s">
+        <v>170</v>
+      </c>
+      <c r="T20" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="U20" s="63" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="73"/>
+      <c r="B21" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="63" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" s="69"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q21" s="63"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="63"/>
+      <c r="T21" s="63"/>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="73"/>
+      <c r="B22" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" s="69"/>
+      <c r="O22" s="73"/>
+      <c r="P22" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="S22" s="63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="C23" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="69"/>
+      <c r="Q23" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="71"/>
+      <c r="S23" s="71"/>
+      <c r="T23" s="71"/>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="B24" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="P24" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q24" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R24" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S24" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T24" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U24" s="68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="H25" s="69"/>
+      <c r="O25" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="R25" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="S25" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="T25" s="63" t="s">
+        <v>177</v>
+      </c>
+      <c r="U25" s="63" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="73"/>
+      <c r="B26" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="H26" s="69"/>
+      <c r="O26" s="73"/>
+      <c r="P26" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="R26" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="T26" s="63" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="73"/>
+      <c r="B27" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="63" t="s">
+        <v>123</v>
+      </c>
+      <c r="H27" s="69"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="S27" s="63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="C31" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="J31" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="71"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="71"/>
+      <c r="Q31" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R31" s="71"/>
+      <c r="S31" s="71"/>
+      <c r="T31" s="71"/>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="B32" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="K32" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="L32" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="M32" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="N32" t="s">
+        <v>18</v>
+      </c>
+      <c r="P32" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q32" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R32" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S32" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T32" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="H33" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="63"/>
+      <c r="O33" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="R33" s="63"/>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="73"/>
+      <c r="B34" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" s="73"/>
+      <c r="I34" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="J34" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="K34" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="O34" s="73"/>
+      <c r="P34" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="R34" s="63"/>
+      <c r="T34" s="63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="73"/>
+      <c r="B35" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="H35" s="73"/>
+      <c r="I35" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="J35" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="K35" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="O35" s="73"/>
+      <c r="P35" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q35" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="R35" s="63"/>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="C37" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="J37" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37" s="71"/>
+      <c r="L37" s="71"/>
+      <c r="M37" s="71"/>
+      <c r="Q37" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R37" s="71"/>
+      <c r="S37" s="71"/>
+      <c r="T37" s="71"/>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="B38" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="J38" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="K38" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="L38" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="M38" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="N38" t="s">
+        <v>18</v>
+      </c>
+      <c r="P38" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q38" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R38" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S38" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T38" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="63"/>
+      <c r="H39" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="K39" s="63"/>
+      <c r="O39" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P39" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="R39" s="63"/>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40" s="73"/>
+      <c r="B40" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="H40" s="73"/>
+      <c r="I40" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="K40" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="O40" s="73"/>
+      <c r="P40" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="R40" s="74"/>
+      <c r="S40" s="63" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" s="73"/>
+      <c r="B41" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" s="73"/>
+      <c r="I41" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="J41" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="O41" s="73"/>
+      <c r="P41" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q41" s="63"/>
+      <c r="S41" s="63" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="C43" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
+      <c r="J43" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="K43" s="71"/>
+      <c r="L43" s="71"/>
+      <c r="M43" s="71"/>
+      <c r="Q43" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R43" s="71"/>
+      <c r="S43" s="71"/>
+      <c r="T43" s="71"/>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="B44" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="J44" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="K44" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="L44" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="M44" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="N44" t="s">
+        <v>18</v>
+      </c>
+      <c r="P44" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q44" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R44" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S44" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T44" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="F45" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="G45" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="H45" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="J45" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="K45" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="M45" s="63" t="s">
+        <v>143</v>
+      </c>
+      <c r="N45" s="63" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="C18" s="66" t="s">
+      <c r="O45" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P45" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q45" s="63" t="s">
+        <v>179</v>
+      </c>
+      <c r="R45" s="63"/>
+      <c r="T45" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="U45" s="63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
+      <c r="A46" s="73"/>
+      <c r="B46" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="E46" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="H46" s="73"/>
+      <c r="I46" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="L46" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="O46" s="73"/>
+      <c r="P46" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="S46" s="63"/>
+    </row>
+    <row r="47" spans="1:21">
+      <c r="A47" s="73"/>
+      <c r="B47" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="H47" s="73"/>
+      <c r="I47" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="J47" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="K47" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="O47" s="73"/>
+      <c r="P47" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q47" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="R47" s="63"/>
+    </row>
+    <row r="49" spans="1:21">
+      <c r="C49" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="B19" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D49" s="71"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="71"/>
+      <c r="J49" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="K49" s="71"/>
+      <c r="L49" s="71"/>
+      <c r="M49" s="71"/>
+      <c r="Q49" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R49" s="71"/>
+      <c r="S49" s="71"/>
+      <c r="T49" s="71"/>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="B50" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E50" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F50" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G50" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="J50" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="K50" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="L50" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="M50" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="N50" t="s">
+        <v>18</v>
+      </c>
+      <c r="P50" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q50" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R50" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S50" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T50" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U50" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
+      <c r="A51" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="F19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="66" t="s">
+      <c r="C51" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="G51" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="H51" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
+      <c r="I51" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="J51" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="K51" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="M51" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="N51" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="O51" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P51" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q51" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="R51" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="T51" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="U51" s="63" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
+      <c r="A52" s="73"/>
+      <c r="B52" s="68" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="66"/>
-      <c r="B21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="C23" s="66" t="s">
+      <c r="H52" s="73"/>
+      <c r="I52" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="O52" s="73"/>
+      <c r="P52" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q52" s="63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
+      <c r="A53" s="73"/>
+      <c r="B53" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="H53" s="73"/>
+      <c r="I53" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="J53" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="K53" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="O53" s="73"/>
+      <c r="P53" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q53" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="R53" s="63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21">
+      <c r="A55" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="B24" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D55" s="71"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="71"/>
+      <c r="H55" t="s">
+        <v>133</v>
+      </c>
+      <c r="J55" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="K55" s="71"/>
+      <c r="L55" s="71"/>
+      <c r="M55" s="71"/>
+      <c r="O55" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q55" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R55" s="71"/>
+      <c r="S55" s="71"/>
+      <c r="T55" s="71"/>
+    </row>
+    <row r="56" spans="1:21">
+      <c r="B56" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E56" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F56" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G56" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="J56" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="K56" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="L56" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="M56" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="N56" t="s">
+        <v>18</v>
+      </c>
+      <c r="P56" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q56" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R56" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S56" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T56" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21">
+      <c r="A57" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="68" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="66" t="s">
+      <c r="D57" s="63"/>
+      <c r="H57" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B25" t="s">
+      <c r="I57" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="K57" s="63"/>
+      <c r="O57" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P57" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="R57" s="63"/>
+      <c r="T57" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="U57" s="63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21">
+      <c r="A58" s="73"/>
+      <c r="B58" s="68" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="66"/>
-      <c r="B26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>104</v>
+      <c r="C58" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="H58" s="73"/>
+      <c r="I58" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="J58" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="L58" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="O58" s="73"/>
+      <c r="P58" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q58" s="63"/>
+      <c r="S58" s="63"/>
+    </row>
+    <row r="59" spans="1:21">
+      <c r="A59" s="73"/>
+      <c r="B59" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="63"/>
+      <c r="H59" s="73"/>
+      <c r="I59" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="J59" s="63"/>
+      <c r="O59" s="73"/>
+      <c r="P59" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q59" s="63" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21">
+      <c r="A60" t="s">
+        <v>135</v>
+      </c>
+      <c r="H60" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21">
+      <c r="C61" s="69"/>
+      <c r="D61" s="69"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="69"/>
+      <c r="Q61" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R61" s="71"/>
+      <c r="S61" s="71"/>
+      <c r="T61" s="71"/>
+    </row>
+    <row r="62" spans="1:21">
+      <c r="P62" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q62" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="R62" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="S62" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="T62" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21">
+      <c r="A63" s="69"/>
+      <c r="O63" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="P63" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="R63" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="T63" s="63"/>
+      <c r="U63" s="63"/>
+    </row>
+    <row r="64" spans="1:21">
+      <c r="A64" s="69"/>
+      <c r="O64" s="73"/>
+      <c r="P64" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q64" s="63"/>
+      <c r="R64" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="S64" s="63"/>
+    </row>
+    <row r="65" spans="1:18">
+      <c r="A65" s="69"/>
+      <c r="O65" s="73"/>
+      <c r="P65" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q65" s="63"/>
+      <c r="R65" s="63" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="A15:A16"/>
+  <mergeCells count="55">
+    <mergeCell ref="X3:AA3"/>
+    <mergeCell ref="V5:V7"/>
+    <mergeCell ref="Q61:T61"/>
+    <mergeCell ref="O63:O65"/>
+    <mergeCell ref="O45:O47"/>
+    <mergeCell ref="Q49:T49"/>
+    <mergeCell ref="O51:O53"/>
+    <mergeCell ref="Q55:T55"/>
+    <mergeCell ref="O57:O59"/>
+    <mergeCell ref="Q31:T31"/>
+    <mergeCell ref="O33:O35"/>
+    <mergeCell ref="Q37:T37"/>
+    <mergeCell ref="O39:O41"/>
+    <mergeCell ref="Q43:T43"/>
+    <mergeCell ref="O15:O17"/>
+    <mergeCell ref="Q18:T18"/>
+    <mergeCell ref="O20:O22"/>
+    <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="O25:O27"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="H45:H47"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="H57:H59"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>